<commit_message>
recommend update and blogs
</commit_message>
<xml_diff>
--- a/src/services/data/interaction_scores.xlsx
+++ b/src/services/data/interaction_scores.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -435,13 +435,13 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B3" t="str">
-        <v>67239b1c63f7c7911db7faaf</v>
+        <v>6728e8a8071b8fcf4f501df0</v>
       </c>
       <c r="C3">
-        <v>0.76</v>
+        <v>0.7</v>
       </c>
       <c r="D3" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-02-12T11:31:56.846Z</v>
       </c>
     </row>
     <row r="4">
@@ -449,13 +449,13 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B4" t="str">
-        <v>6728e8a8071b8fcf4f501df0</v>
+        <v>6728e9ab071b8fcf4f501df6</v>
       </c>
       <c r="C4">
-        <v>0.7</v>
+        <v>0.88</v>
       </c>
       <c r="D4" t="str">
-        <v>2025-02-12T11:31:56.846Z</v>
+        <v>2025-04-13T11:31:56.846Z</v>
       </c>
     </row>
     <row r="5">
@@ -463,10 +463,10 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B5" t="str">
-        <v>6728e9ab071b8fcf4f501df6</v>
+        <v>6728e9e6071b8fcf4f501dfc</v>
       </c>
       <c r="C5">
-        <v>0.88</v>
+        <v>0.94</v>
       </c>
       <c r="D5" t="str">
         <v>2025-04-13T11:31:56.846Z</v>
@@ -477,10 +477,10 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B6" t="str">
-        <v>6728e9e6071b8fcf4f501dfc</v>
+        <v>6728ea62071b8fcf4f501e02</v>
       </c>
       <c r="C6">
-        <v>0.94</v>
+        <v>0.82</v>
       </c>
       <c r="D6" t="str">
         <v>2025-04-13T11:31:56.846Z</v>
@@ -491,7 +491,7 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B7" t="str">
-        <v>6728ea62071b8fcf4f501e02</v>
+        <v>6743a3a8fd3ceed5b16a5e18</v>
       </c>
       <c r="C7">
         <v>0.82</v>
@@ -505,10 +505,10 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B8" t="str">
-        <v>6743a3a8fd3ceed5b16a5e18</v>
+        <v>676137906c06138b1419f8a5</v>
       </c>
       <c r="C8">
-        <v>0.82</v>
+        <v>0.94</v>
       </c>
       <c r="D8" t="str">
         <v>2025-04-13T11:31:56.846Z</v>
@@ -519,10 +519,10 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B9" t="str">
-        <v>676137906c06138b1419f8a5</v>
+        <v>67f08cab1841d535b6af6f50</v>
       </c>
       <c r="C9">
-        <v>0.94</v>
+        <v>0.76</v>
       </c>
       <c r="D9" t="str">
         <v>2025-04-13T11:31:56.846Z</v>
@@ -533,10 +533,10 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B10" t="str">
-        <v>67f08cab1841d535b6af6f50</v>
+        <v>67f08e231841d535b6af6f67</v>
       </c>
       <c r="C10">
-        <v>0.76</v>
+        <v>0.82</v>
       </c>
       <c r="D10" t="str">
         <v>2025-04-13T11:31:56.846Z</v>
@@ -547,13 +547,13 @@
         <v>6739a4c617dc7ef140b34295</v>
       </c>
       <c r="B11" t="str">
-        <v>67f08e231841d535b6af6f67</v>
+        <v>6728eb4a071b8fcf4f501e0b</v>
       </c>
       <c r="C11">
-        <v>0.82</v>
+        <v>0.76</v>
       </c>
       <c r="D11" t="str">
-        <v>2025-04-13T11:31:56.846Z</v>
+        <v>2025-05-23T04:46:31.245Z</v>
       </c>
     </row>
     <row r="12">
@@ -1060,9 +1060,107 @@
         <v>2025-03-12T11:31:56.846Z</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B48" t="str">
+        <v>6728e9e6071b8fcf4f501dfc</v>
+      </c>
+      <c r="C48">
+        <v>0.925</v>
+      </c>
+      <c r="D48" t="str">
+        <v>2025-05-23T04:41:14.096Z</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B49" t="str">
+        <v>6728e93a071b8fcf4f501df3</v>
+      </c>
+      <c r="C49">
+        <v>0.775</v>
+      </c>
+      <c r="D49" t="str">
+        <v>2025-05-23T09:19:25.598Z</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B50" t="str">
+        <v>6728ea18071b8fcf4f501dff</v>
+      </c>
+      <c r="C50">
+        <v>0.775</v>
+      </c>
+      <c r="D50" t="str">
+        <v>2025-05-23T09:19:36.004Z</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B51" t="str">
+        <v>67f091181841d535b6af6f7b</v>
+      </c>
+      <c r="C51">
+        <v>0.775</v>
+      </c>
+      <c r="D51" t="str">
+        <v>2025-05-23T09:19:59.350Z</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B52" t="str">
+        <v>6728e9cd071b8fcf4f501df9</v>
+      </c>
+      <c r="C52">
+        <v>0.925</v>
+      </c>
+      <c r="D52" t="str">
+        <v>2025-05-23T09:21:52.485Z</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B53" t="str">
+        <v>6728f96acb86d3695fa1f4a6</v>
+      </c>
+      <c r="C53">
+        <v>0.775</v>
+      </c>
+      <c r="D53" t="str">
+        <v>2025-05-23T09:21:00.865Z</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B54" t="str">
+        <v>68067dd1286f80e4174d8736</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="str">
+        <v>2025-05-23T09:23:22.245Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D47"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D54"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(back-end): intergrate finding with gemini
</commit_message>
<xml_diff>
--- a/src/services/data/interaction_scores.xlsx
+++ b/src/services/data/interaction_scores.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -830,7 +830,7 @@
         <v>67447fbced2b056beb0f8e01</v>
       </c>
       <c r="C31">
-        <v>0.94</v>
+        <v>0.7</v>
       </c>
       <c r="D31" t="str">
         <v>2025-03-12T11:31:56.846Z</v>
@@ -886,7 +886,7 @@
         <v>6728ea62071b8fcf4f501e02</v>
       </c>
       <c r="C35">
-        <v>0.86</v>
+        <v>0.7</v>
       </c>
       <c r="D35" t="str">
         <v>2025-03-12T11:31:56.846Z</v>
@@ -942,7 +942,7 @@
         <v>6728ea18071b8fcf4f501dff</v>
       </c>
       <c r="C39">
-        <v>0.84</v>
+        <v>0.7</v>
       </c>
       <c r="D39" t="str">
         <v>2025-03-12T11:31:56.846Z</v>
@@ -967,13 +967,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B41" t="str">
-        <v>6728e8a8071b8fcf4f501df0</v>
+        <v>67f095081841d535b6af6fae</v>
       </c>
       <c r="C41">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="D41" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T04:37:38.841Z</v>
       </c>
     </row>
     <row r="42">
@@ -981,13 +981,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B42" t="str">
-        <v>6728e93a071b8fcf4f501df3</v>
+        <v>67f093ce1841d535b6af6f93</v>
       </c>
       <c r="C42">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="D42" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T04:38:31.695Z</v>
       </c>
     </row>
     <row r="43">
@@ -995,13 +995,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B43" t="str">
-        <v>6728e9cd071b8fcf4f501df9</v>
+        <v>67f0959c1841d535b6af6fb4</v>
       </c>
       <c r="C43">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="D43" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T04:49:13.113Z</v>
       </c>
     </row>
     <row r="44">
@@ -1009,13 +1009,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B44" t="str">
-        <v>6728eb84071b8fcf4f501e0e</v>
+        <v>67f094ec1841d535b6af6fab</v>
       </c>
       <c r="C44">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="D44" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T04:52:37.819Z</v>
       </c>
     </row>
     <row r="45">
@@ -1023,13 +1023,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B45" t="str">
-        <v>6728ebe1071b8fcf4f501e14</v>
+        <v>6728e9cd071b8fcf4f501df9</v>
       </c>
       <c r="C45">
-        <v>0.26</v>
+        <v>0.1</v>
       </c>
       <c r="D45" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T04:53:07.969Z</v>
       </c>
     </row>
     <row r="46">
@@ -1037,13 +1037,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B46" t="str">
-        <v>6728f96acb86d3695fa1f4a6</v>
+        <v>67f095dc1841d535b6af6fba</v>
       </c>
       <c r="C46">
-        <v>0.22</v>
+        <v>0.1</v>
       </c>
       <c r="D46" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T05:24:22.234Z</v>
       </c>
     </row>
     <row r="47">
@@ -1051,55 +1051,55 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B47" t="str">
-        <v>6742f65b3a89ce4d5d1c475a</v>
+        <v>67f094111841d535b6af6f99</v>
       </c>
       <c r="C47">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="D47" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T05:27:27.719Z</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>682326702fff19d415752f01</v>
+        <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B48" t="str">
-        <v>6728e9e6071b8fcf4f501dfc</v>
+        <v>67f092321841d535b6af6f81</v>
       </c>
       <c r="C48">
-        <v>0.925</v>
+        <v>0.3</v>
       </c>
       <c r="D48" t="str">
-        <v>2025-05-23T04:41:14.096Z</v>
+        <v>2025-06-01T05:45:55.487Z</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>682326702fff19d415752f01</v>
+        <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B49" t="str">
-        <v>6728e93a071b8fcf4f501df3</v>
+        <v>6728e8a8071b8fcf4f501df0</v>
       </c>
       <c r="C49">
-        <v>0.775</v>
+        <v>0.1</v>
       </c>
       <c r="D49" t="str">
-        <v>2025-05-23T09:19:25.598Z</v>
+        <v>2025-06-01T06:14:02.581Z</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>682326702fff19d415752f01</v>
+        <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B50" t="str">
-        <v>6728ea18071b8fcf4f501dff</v>
+        <v>67f095371841d535b6af6fb1</v>
       </c>
       <c r="C50">
-        <v>0.775</v>
+        <v>0.3</v>
       </c>
       <c r="D50" t="str">
-        <v>2025-05-23T09:19:36.004Z</v>
+        <v>2025-06-01T06:15:38.184Z</v>
       </c>
     </row>
     <row r="51">
@@ -1107,13 +1107,13 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B51" t="str">
-        <v>67f091181841d535b6af6f7b</v>
+        <v>6728e9e6071b8fcf4f501dfc</v>
       </c>
       <c r="C51">
-        <v>0.775</v>
+        <v>0.925</v>
       </c>
       <c r="D51" t="str">
-        <v>2025-05-23T09:19:59.350Z</v>
+        <v>2025-05-23T04:41:14.096Z</v>
       </c>
     </row>
     <row r="52">
@@ -1121,13 +1121,13 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B52" t="str">
-        <v>6728e9cd071b8fcf4f501df9</v>
+        <v>6728e93a071b8fcf4f501df3</v>
       </c>
       <c r="C52">
-        <v>0.925</v>
+        <v>0.775</v>
       </c>
       <c r="D52" t="str">
-        <v>2025-05-23T09:21:52.485Z</v>
+        <v>2025-05-23T09:19:25.598Z</v>
       </c>
     </row>
     <row r="53">
@@ -1135,13 +1135,13 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B53" t="str">
-        <v>6728f96acb86d3695fa1f4a6</v>
+        <v>6728ea18071b8fcf4f501dff</v>
       </c>
       <c r="C53">
         <v>0.775</v>
       </c>
       <c r="D53" t="str">
-        <v>2025-05-23T09:21:00.865Z</v>
+        <v>2025-05-23T09:19:36.004Z</v>
       </c>
     </row>
     <row r="54">
@@ -1149,46 +1149,116 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B54" t="str">
-        <v>68067dd1286f80e4174d8736</v>
+        <v>67f091181841d535b6af6f7b</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0.775</v>
       </c>
       <c r="D54" t="str">
-        <v>2025-05-23T09:23:22.245Z</v>
+        <v>2025-05-23T09:19:59.350Z</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>683b37622eb85e2df9802771</v>
+        <v>682326702fff19d415752f01</v>
       </c>
       <c r="B55" t="str">
-        <v>6728e93a071b8fcf4f501df3</v>
+        <v>6728e9cd071b8fcf4f501df9</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0.925</v>
       </c>
       <c r="D55" t="str">
-        <v>2025-05-31T17:08:32.178Z</v>
+        <v>2025-05-23T09:21:52.485Z</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B56" t="str">
+        <v>6728f96acb86d3695fa1f4a6</v>
+      </c>
+      <c r="C56">
+        <v>0.775</v>
+      </c>
+      <c r="D56" t="str">
+        <v>2025-05-23T09:21:00.865Z</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B57" t="str">
+        <v>68067dd1286f80e4174d8736</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <v>2025-05-23T09:23:22.245Z</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
         <v>683b37622eb85e2df9802771</v>
       </c>
-      <c r="B56" t="str">
+      <c r="B58" t="str">
+        <v>6728e93a071b8fcf4f501df3</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <v>2025-05-31T17:08:32.178Z</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>683b37622eb85e2df9802771</v>
+      </c>
+      <c r="B59" t="str">
         <v>6728ea18071b8fcf4f501dff</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>0.85</v>
       </c>
-      <c r="D56" t="str">
+      <c r="D59" t="str">
         <v>2025-05-31T17:10:43.229Z</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>683b37622eb85e2df9802771</v>
+      </c>
+      <c r="B60" t="str">
+        <v>6728f96acb86d3695fa1f4a6</v>
+      </c>
+      <c r="C60">
+        <v>0.15</v>
+      </c>
+      <c r="D60" t="str">
+        <v>2025-06-01T02:53:50.928Z</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>683b37622eb85e2df9802771</v>
+      </c>
+      <c r="B61" t="str">
+        <v>6728ec07071b8fcf4f501e17</v>
+      </c>
+      <c r="C61">
+        <v>0.15</v>
+      </c>
+      <c r="D61" t="str">
+        <v>2025-06-01T07:31:20.015Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D56"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D61"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update info and payment
</commit_message>
<xml_diff>
--- a/src/services/data/interaction_scores.xlsx
+++ b/src/services/data/interaction_scores.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -830,7 +830,7 @@
         <v>67447fbced2b056beb0f8e01</v>
       </c>
       <c r="C31">
-        <v>0.94</v>
+        <v>0.7</v>
       </c>
       <c r="D31" t="str">
         <v>2025-03-12T11:31:56.846Z</v>
@@ -886,7 +886,7 @@
         <v>6728ea62071b8fcf4f501e02</v>
       </c>
       <c r="C35">
-        <v>0.86</v>
+        <v>0.7</v>
       </c>
       <c r="D35" t="str">
         <v>2025-03-12T11:31:56.846Z</v>
@@ -942,7 +942,7 @@
         <v>6728ea18071b8fcf4f501dff</v>
       </c>
       <c r="C39">
-        <v>0.84</v>
+        <v>0.7</v>
       </c>
       <c r="D39" t="str">
         <v>2025-03-12T11:31:56.846Z</v>
@@ -967,13 +967,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B41" t="str">
-        <v>6728e8a8071b8fcf4f501df0</v>
+        <v>67f0959c1841d535b6af6fb4</v>
       </c>
       <c r="C41">
-        <v>0.06</v>
+        <v>0.15</v>
       </c>
       <c r="D41" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T04:49:13.113Z</v>
       </c>
     </row>
     <row r="42">
@@ -981,13 +981,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B42" t="str">
-        <v>6728e93a071b8fcf4f501df3</v>
+        <v>67f094ec1841d535b6af6fab</v>
       </c>
       <c r="C42">
-        <v>0.3</v>
+        <v>0.075</v>
       </c>
       <c r="D42" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T04:52:37.819Z</v>
       </c>
     </row>
     <row r="43">
@@ -998,10 +998,10 @@
         <v>6728e9cd071b8fcf4f501df9</v>
       </c>
       <c r="C43">
-        <v>0.24</v>
+        <v>0.225</v>
       </c>
       <c r="D43" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T09:00:07.871Z</v>
       </c>
     </row>
     <row r="44">
@@ -1009,13 +1009,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B44" t="str">
-        <v>6728eb84071b8fcf4f501e0e</v>
+        <v>67f095dc1841d535b6af6fba</v>
       </c>
       <c r="C44">
-        <v>0.08</v>
+        <v>0.075</v>
       </c>
       <c r="D44" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T05:24:22.234Z</v>
       </c>
     </row>
     <row r="45">
@@ -1023,13 +1023,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B45" t="str">
-        <v>6728ebe1071b8fcf4f501e14</v>
+        <v>67f094111841d535b6af6f99</v>
       </c>
       <c r="C45">
-        <v>0.26</v>
+        <v>0.075</v>
       </c>
       <c r="D45" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T05:27:27.719Z</v>
       </c>
     </row>
     <row r="46">
@@ -1037,13 +1037,13 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B46" t="str">
-        <v>6728f96acb86d3695fa1f4a6</v>
+        <v>67f092321841d535b6af6f81</v>
       </c>
       <c r="C46">
-        <v>0.22</v>
+        <v>0.225</v>
       </c>
       <c r="D46" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T05:45:55.487Z</v>
       </c>
     </row>
     <row r="47">
@@ -1051,55 +1051,55 @@
         <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B47" t="str">
-        <v>6742f65b3a89ce4d5d1c475a</v>
+        <v>6728e8a8071b8fcf4f501df0</v>
       </c>
       <c r="C47">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="D47" t="str">
-        <v>2025-03-12T11:31:56.846Z</v>
+        <v>2025-06-01T07:32:49.957Z</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>682326702fff19d415752f01</v>
+        <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B48" t="str">
-        <v>6728e9e6071b8fcf4f501dfc</v>
+        <v>67f095371841d535b6af6fb1</v>
       </c>
       <c r="C48">
-        <v>0.925</v>
+        <v>0.3</v>
       </c>
       <c r="D48" t="str">
-        <v>2025-05-23T04:41:14.096Z</v>
+        <v>2025-06-01T07:48:03.296Z</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>682326702fff19d415752f01</v>
+        <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B49" t="str">
-        <v>6728e93a071b8fcf4f501df3</v>
+        <v>6728ec07071b8fcf4f501e17</v>
       </c>
       <c r="C49">
-        <v>0.775</v>
+        <v>0.075</v>
       </c>
       <c r="D49" t="str">
-        <v>2025-05-23T09:19:25.598Z</v>
+        <v>2025-06-01T07:57:47.828Z</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>682326702fff19d415752f01</v>
+        <v>6738b019504ed0629a25b8b1</v>
       </c>
       <c r="B50" t="str">
-        <v>6728ea18071b8fcf4f501dff</v>
+        <v>6728ebe1071b8fcf4f501e14</v>
       </c>
       <c r="C50">
-        <v>0.775</v>
+        <v>0.225</v>
       </c>
       <c r="D50" t="str">
-        <v>2025-05-23T09:19:36.004Z</v>
+        <v>2025-06-02T01:19:45.553Z</v>
       </c>
     </row>
     <row r="51">
@@ -1107,13 +1107,13 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B51" t="str">
-        <v>67f091181841d535b6af6f7b</v>
+        <v>6728e9e6071b8fcf4f501dfc</v>
       </c>
       <c r="C51">
-        <v>0.775</v>
+        <v>0.925</v>
       </c>
       <c r="D51" t="str">
-        <v>2025-05-23T09:19:59.350Z</v>
+        <v>2025-05-23T04:41:14.096Z</v>
       </c>
     </row>
     <row r="52">
@@ -1121,13 +1121,13 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B52" t="str">
-        <v>6728e9cd071b8fcf4f501df9</v>
+        <v>6728e93a071b8fcf4f501df3</v>
       </c>
       <c r="C52">
-        <v>0.925</v>
+        <v>0.775</v>
       </c>
       <c r="D52" t="str">
-        <v>2025-05-23T09:21:52.485Z</v>
+        <v>2025-05-23T09:19:25.598Z</v>
       </c>
     </row>
     <row r="53">
@@ -1135,13 +1135,13 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B53" t="str">
-        <v>6728f96acb86d3695fa1f4a6</v>
+        <v>6728ea18071b8fcf4f501dff</v>
       </c>
       <c r="C53">
         <v>0.775</v>
       </c>
       <c r="D53" t="str">
-        <v>2025-05-23T09:21:00.865Z</v>
+        <v>2025-05-23T09:19:36.004Z</v>
       </c>
     </row>
     <row r="54">
@@ -1149,46 +1149,116 @@
         <v>682326702fff19d415752f01</v>
       </c>
       <c r="B54" t="str">
-        <v>68067dd1286f80e4174d8736</v>
+        <v>67f091181841d535b6af6f7b</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0.775</v>
       </c>
       <c r="D54" t="str">
-        <v>2025-05-23T09:23:22.245Z</v>
+        <v>2025-05-23T09:19:59.350Z</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>683b37622eb85e2df9802771</v>
+        <v>682326702fff19d415752f01</v>
       </c>
       <c r="B55" t="str">
-        <v>6728e93a071b8fcf4f501df3</v>
+        <v>6728e9cd071b8fcf4f501df9</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>0.925</v>
       </c>
       <c r="D55" t="str">
-        <v>2025-05-31T17:08:32.178Z</v>
+        <v>2025-05-23T09:21:52.485Z</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B56" t="str">
+        <v>6728f96acb86d3695fa1f4a6</v>
+      </c>
+      <c r="C56">
+        <v>0.775</v>
+      </c>
+      <c r="D56" t="str">
+        <v>2025-05-23T09:21:00.865Z</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>682326702fff19d415752f01</v>
+      </c>
+      <c r="B57" t="str">
+        <v>68067dd1286f80e4174d8736</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57" t="str">
+        <v>2025-05-23T09:23:22.245Z</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
         <v>683b37622eb85e2df9802771</v>
       </c>
-      <c r="B56" t="str">
+      <c r="B58" t="str">
+        <v>6728e93a071b8fcf4f501df3</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" t="str">
+        <v>2025-05-31T17:08:32.178Z</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>683b37622eb85e2df9802771</v>
+      </c>
+      <c r="B59" t="str">
         <v>6728ea18071b8fcf4f501dff</v>
       </c>
-      <c r="C56">
+      <c r="C59">
         <v>0.85</v>
       </c>
-      <c r="D56" t="str">
+      <c r="D59" t="str">
         <v>2025-05-31T17:10:43.229Z</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>683b37622eb85e2df9802771</v>
+      </c>
+      <c r="B60" t="str">
+        <v>6728f96acb86d3695fa1f4a6</v>
+      </c>
+      <c r="C60">
+        <v>0.15</v>
+      </c>
+      <c r="D60" t="str">
+        <v>2025-06-01T02:53:50.928Z</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>683b37622eb85e2df9802771</v>
+      </c>
+      <c r="B61" t="str">
+        <v>6728ec07071b8fcf4f501e17</v>
+      </c>
+      <c r="C61">
+        <v>0.15</v>
+      </c>
+      <c r="D61" t="str">
+        <v>2025-06-01T07:31:20.015Z</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D56"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D61"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>